<commit_message>
Adiciona os scripts de inserção e visualização de dados
</commit_message>
<xml_diff>
--- a/Banco de dados/modelagens/SpMedGroup-fisico.xlsx
+++ b/Banco de dados/modelagens/SpMedGroup-fisico.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
   <si>
     <t>tipoUsuario</t>
   </si>
@@ -84,9 +84,6 @@
     <t>SP Medical Group</t>
   </si>
   <si>
-    <t>86.400.902/0001-30</t>
-  </si>
-  <si>
     <t>especialidade</t>
   </si>
   <si>
@@ -276,45 +273,21 @@
     <t>Ligia</t>
   </si>
   <si>
-    <t>43522543-5</t>
-  </si>
-  <si>
     <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
   </si>
   <si>
     <t>10/13/1983</t>
   </si>
   <si>
-    <t>11 3456-7654</t>
-  </si>
-  <si>
     <t>Alexandre</t>
   </si>
   <si>
-    <t>32654345-7</t>
-  </si>
-  <si>
     <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
   </si>
   <si>
     <t>7/23/2001</t>
   </si>
   <si>
-    <t>11 98765-6543</t>
-  </si>
-  <si>
-    <t>11 97208-4453</t>
-  </si>
-  <si>
-    <t>11 3456-6543</t>
-  </si>
-  <si>
-    <t>11 7656-6377</t>
-  </si>
-  <si>
-    <t>11 95436-8769</t>
-  </si>
-  <si>
     <t>Fernando</t>
   </si>
   <si>
@@ -330,21 +303,6 @@
     <t>Mariana</t>
   </si>
   <si>
-    <t>54636525-3</t>
-  </si>
-  <si>
-    <t>54366362-5</t>
-  </si>
-  <si>
-    <t>53254444-1</t>
-  </si>
-  <si>
-    <t>54566266-7</t>
-  </si>
-  <si>
-    <t>54566266-8</t>
-  </si>
-  <si>
     <t>Av. Ibirapuera - Indianópolis, 2927,  São Paulo - SP, 04029-200</t>
   </si>
   <si>
@@ -390,15 +348,6 @@
     <t>Helena Strada</t>
   </si>
   <si>
-    <t>54356-SP</t>
-  </si>
-  <si>
-    <t>53452-SP</t>
-  </si>
-  <si>
-    <t>65463-SP</t>
-  </si>
-  <si>
     <t>consulta</t>
   </si>
   <si>
@@ -412,6 +361,15 @@
   </si>
   <si>
     <t>1/20/20 15:00</t>
+  </si>
+  <si>
+    <t>54356SP</t>
+  </si>
+  <si>
+    <t>53452SP</t>
+  </si>
+  <si>
+    <t>65463SP</t>
   </si>
 </sst>
 </file>
@@ -481,13 +439,7 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -502,6 +454,12 @@
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -513,24 +471,32 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -878,96 +844,60 @@
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
@@ -1127,6 +1057,34 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1255,109 +1213,109 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:B5" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:B5" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A2:B5"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idTipoUsuario" dataDxfId="52"/>
-    <tableColumn id="2" name="nomeTipoUsuario" dataDxfId="51"/>
+    <tableColumn id="1" name="idTipoUsuario" dataDxfId="50"/>
+    <tableColumn id="2" name="nomeTipoUsuario" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:G3" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A2:G3" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="A2:G3"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="idClinica" dataDxfId="48"/>
-    <tableColumn id="2" name="endClinica" dataDxfId="47"/>
-    <tableColumn id="3" name="nomeFantasia" dataDxfId="46"/>
-    <tableColumn id="4" name="razaoSocial" dataDxfId="45"/>
-    <tableColumn id="5" name="horaAbertura" dataDxfId="44"/>
-    <tableColumn id="6" name="horaFechamento" dataDxfId="43"/>
-    <tableColumn id="7" name="cnpj" dataDxfId="42"/>
+    <tableColumn id="1" name="idClinica" dataDxfId="46"/>
+    <tableColumn id="2" name="endClinica" dataDxfId="45"/>
+    <tableColumn id="3" name="nomeFantasia" dataDxfId="44"/>
+    <tableColumn id="4" name="razaoSocial" dataDxfId="43"/>
+    <tableColumn id="5" name="horaAbertura" dataDxfId="42"/>
+    <tableColumn id="6" name="horaFechamento" dataDxfId="41"/>
+    <tableColumn id="7" name="cnpj" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A2:B19" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A2:B19" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A2:B19"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idEspecialidade" dataDxfId="39"/>
-    <tableColumn id="2" name="nomeEspecialidade" dataDxfId="38"/>
+    <tableColumn id="1" name="idEspecialidade" dataDxfId="37"/>
+    <tableColumn id="2" name="nomeEspecialidade" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A2:B5" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A2:B5" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:B5"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="idSituacao" dataDxfId="35"/>
-    <tableColumn id="2" name="situacaoDesc" dataDxfId="34"/>
+    <tableColumn id="1" name="idSituacao" dataDxfId="33"/>
+    <tableColumn id="2" name="situacaoDesc" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A2:D14" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A2:D14" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A2:D14"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="idUsuario" dataDxfId="31"/>
-    <tableColumn id="2" name="idTipoUsuario" dataDxfId="30"/>
-    <tableColumn id="3" name="email" dataDxfId="29" dataCellStyle="Hiperlink"/>
-    <tableColumn id="4" name="senha" dataDxfId="28"/>
+    <tableColumn id="1" name="idUsuario" dataDxfId="29"/>
+    <tableColumn id="2" name="idTipoUsuario" dataDxfId="2"/>
+    <tableColumn id="3" name="email" dataDxfId="0" dataCellStyle="Hiperlink"/>
+    <tableColumn id="4" name="senha" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A2:H9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A2:H9" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:H9"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="idPaciente" dataDxfId="25"/>
-    <tableColumn id="2" name="idUsuario" dataDxfId="24"/>
-    <tableColumn id="3" name="nomePaciente" dataDxfId="23"/>
-    <tableColumn id="4" name="rgPaciente" dataDxfId="22"/>
-    <tableColumn id="5" name="cpfPaciente" dataDxfId="21"/>
-    <tableColumn id="6" name="endPaciente" dataDxfId="20"/>
-    <tableColumn id="7" name="dataNascPaciente" dataDxfId="19"/>
-    <tableColumn id="8" name="telPaciente" dataDxfId="18"/>
+    <tableColumn id="1" name="idPaciente" dataDxfId="26"/>
+    <tableColumn id="2" name="idUsuario" dataDxfId="25"/>
+    <tableColumn id="3" name="nomePaciente" dataDxfId="24"/>
+    <tableColumn id="4" name="rgPaciente" dataDxfId="23"/>
+    <tableColumn id="5" name="cpfPaciente" dataDxfId="22"/>
+    <tableColumn id="6" name="endPaciente" dataDxfId="21"/>
+    <tableColumn id="7" name="dataNascPaciente" dataDxfId="20"/>
+    <tableColumn id="8" name="telPaciente" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A2:F5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A2:F5" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A2:F5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="idMedico" dataDxfId="15"/>
-    <tableColumn id="2" name="idUsuario" dataDxfId="14"/>
-    <tableColumn id="3" name="idClinica" dataDxfId="13"/>
-    <tableColumn id="4" name="idEspecialidade" dataDxfId="12"/>
-    <tableColumn id="5" name="crm" dataDxfId="11"/>
-    <tableColumn id="6" name="nomeMedico" dataDxfId="10"/>
+    <tableColumn id="1" name="idMedico" dataDxfId="16"/>
+    <tableColumn id="2" name="idUsuario" dataDxfId="15"/>
+    <tableColumn id="3" name="idClinica" dataDxfId="14"/>
+    <tableColumn id="4" name="idEspecialidade" dataDxfId="13"/>
+    <tableColumn id="5" name="crm" dataDxfId="12"/>
+    <tableColumn id="6" name="nomeMedico" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A2:F9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela8" displayName="Tabela8" ref="A2:F9" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A2:F9"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="idConsulta" dataDxfId="7"/>
-    <tableColumn id="2" name="idPaciente" dataDxfId="6"/>
-    <tableColumn id="3" name="idMedico" dataDxfId="5"/>
-    <tableColumn id="4" name="idSituacao" dataDxfId="4"/>
-    <tableColumn id="5" name="consultaDesc" dataDxfId="3"/>
-    <tableColumn id="6" name="dataConsulta" dataDxfId="2"/>
+    <tableColumn id="1" name="idConsulta" dataDxfId="8"/>
+    <tableColumn id="2" name="idPaciente" dataDxfId="7"/>
+    <tableColumn id="3" name="idMedico" dataDxfId="6"/>
+    <tableColumn id="4" name="idSituacao" dataDxfId="5"/>
+    <tableColumn id="5" name="consultaDesc" dataDxfId="4"/>
+    <tableColumn id="6" name="dataConsulta" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1639,40 +1597,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1693,7 +1651,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,64 +1662,64 @@
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>0.29166666666666669</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>0.875</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
+      <c r="G3" s="1">
+        <v>86400902000130</v>
       </c>
     </row>
   </sheetData>
@@ -1779,7 +1737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -1790,153 +1748,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1965,41 +1923,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +1976,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,193 +1988,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2237,8 +2195,9 @@
     <hyperlink ref="C14" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2247,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2264,222 +2223,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="D3" s="1">
+        <v>435225435</v>
+      </c>
+      <c r="E3" s="1">
+        <v>94839859000</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1134567654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1">
+        <v>326543457</v>
+      </c>
+      <c r="E4" s="1">
+        <v>73556944057</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="1">
+        <v>11987656543</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="1">
+        <v>546365253</v>
+      </c>
+      <c r="E5" s="1">
+        <v>16839338002</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="4">
+        <v>28773</v>
+      </c>
+      <c r="H5" s="1">
+        <v>11972084453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="1">
+        <v>543663625</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14332654765</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1134566543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="1">
+        <v>532544441</v>
+      </c>
+      <c r="E7" s="1">
+        <v>91305348010</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1176566377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="2">
-        <v>94839859000</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="1">
+        <v>545662667</v>
+      </c>
+      <c r="E8" s="1">
+        <v>79799299004</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="1">
+        <v>11954368769</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="2">
-        <v>73556944057</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D9" s="1">
+        <v>545662668</v>
+      </c>
+      <c r="E9" s="1">
+        <v>13771913039</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="2">
-        <v>16839338002</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="6">
-        <v>28773</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="2">
-        <v>14332654765</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E7" s="2">
-        <v>91305348010</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="2">
-        <v>79799299004</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="2">
-        <v>13771913039</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>43223</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2496,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2511,93 +2470,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>118</v>
+      <c r="F5" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2575,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,158 +2589,158 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="A1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>125</v>
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>126</v>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="7">
+      <c r="E4" s="1"/>
+      <c r="F4" s="5">
         <v>43983.416666666664</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="7">
+      <c r="E5" s="1"/>
+      <c r="F5" s="5">
         <v>44014.458333333336</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="7">
+      <c r="E6" s="1"/>
+      <c r="F6" s="5">
         <v>43253.416666666664</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="7">
+      <c r="E7" s="1"/>
+      <c r="F7" s="5">
         <v>43648.458333333336</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7">
+      <c r="E8" s="1"/>
+      <c r="F8" s="5">
         <v>44046.625</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="7">
+      <c r="E9" s="1"/>
+      <c r="F9" s="5">
         <v>44077.458333333336</v>
       </c>
     </row>

</xml_diff>